<commit_message>
fixed error in blackspots file
</commit_message>
<xml_diff>
--- a/All Blackspots.xlsx
+++ b/All Blackspots.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="560" yWindow="460" windowWidth="24720" windowHeight="15540" tabRatio="500"/>
+    <workbookView xWindow="880" yWindow="460" windowWidth="24720" windowHeight="15540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -772,8 +772,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N531"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="O82" sqref="O82"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A139" workbookViewId="0">
+      <selection activeCell="F156" sqref="F156"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7145,6 +7145,9 @@
       <c r="B156" s="2">
         <v>151.23110109999999</v>
       </c>
+      <c r="C156" s="2">
+        <v>1271</v>
+      </c>
       <c r="D156" s="2">
         <v>3</v>
       </c>
@@ -7184,7 +7187,7 @@
         <v>151.23109819999999</v>
       </c>
       <c r="C157" s="2">
-        <v>1271</v>
+        <v>1309</v>
       </c>
       <c r="D157" s="2">
         <v>7</v>
@@ -7225,7 +7228,7 @@
         <v>151.23109400000001</v>
       </c>
       <c r="C158" s="2">
-        <v>1309</v>
+        <v>1424</v>
       </c>
       <c r="D158" s="2">
         <v>11</v>
@@ -7266,7 +7269,7 @@
         <v>151.23108479999999</v>
       </c>
       <c r="C159" s="2">
-        <v>1424</v>
+        <v>1439</v>
       </c>
       <c r="D159" s="2">
         <v>13</v>
@@ -7307,7 +7310,7 @@
         <v>151.23107920000001</v>
       </c>
       <c r="C160" s="2">
-        <v>1439</v>
+        <v>1341</v>
       </c>
       <c r="D160" s="2">
         <v>16</v>
@@ -7348,7 +7351,7 @@
         <v>151.23108049999999</v>
       </c>
       <c r="C161" s="2">
-        <v>1341</v>
+        <v>1314</v>
       </c>
       <c r="D161" s="2">
         <v>11</v>
@@ -7389,7 +7392,7 @@
         <v>151.23108010000001</v>
       </c>
       <c r="C162" s="2">
-        <v>1314</v>
+        <v>1394</v>
       </c>
       <c r="D162" s="2">
         <v>10</v>
@@ -7430,7 +7433,7 @@
         <v>151.23107970000001</v>
       </c>
       <c r="C163" s="2">
-        <v>1394</v>
+        <v>1310</v>
       </c>
       <c r="D163" s="2">
         <v>11</v>
@@ -7471,7 +7474,7 @@
         <v>151.23107920000001</v>
       </c>
       <c r="C164" s="2">
-        <v>1310</v>
+        <v>5509</v>
       </c>
       <c r="D164" s="2">
         <v>11</v>
@@ -7512,7 +7515,7 @@
         <v>151.23107899999999</v>
       </c>
       <c r="C165" s="2">
-        <v>5509</v>
+        <v>1282</v>
       </c>
       <c r="D165" s="2">
         <v>11</v>
@@ -7553,7 +7556,7 @@
         <v>151.23107949999999</v>
       </c>
       <c r="C166" s="2">
-        <v>1282</v>
+        <v>1291</v>
       </c>
       <c r="D166" s="2">
         <v>11</v>
@@ -7594,7 +7597,7 @@
         <v>151.2310794</v>
       </c>
       <c r="C167" s="2">
-        <v>1291</v>
+        <v>1300</v>
       </c>
       <c r="D167" s="2">
         <v>11</v>
@@ -7635,7 +7638,7 @@
         <v>151.23107920000001</v>
       </c>
       <c r="C168" s="2">
-        <v>1300</v>
+        <v>1304</v>
       </c>
       <c r="D168" s="2">
         <v>11</v>
@@ -7676,7 +7679,7 @@
         <v>151.23107909999999</v>
       </c>
       <c r="C169" s="2">
-        <v>1304</v>
+        <v>1338</v>
       </c>
       <c r="D169" s="2">
         <v>12</v>
@@ -7717,7 +7720,7 @@
         <v>151.2310765</v>
       </c>
       <c r="C170" s="2">
-        <v>1338</v>
+        <v>1759</v>
       </c>
       <c r="D170" s="2">
         <v>13</v>
@@ -7758,7 +7761,7 @@
         <v>151.23095520000001</v>
       </c>
       <c r="C171" s="2">
-        <v>1759</v>
+        <v>1685</v>
       </c>
       <c r="D171" s="2">
         <v>9</v>
@@ -7799,7 +7802,7 @@
         <v>151.23101729999999</v>
       </c>
       <c r="C172" s="2">
-        <v>1685</v>
+        <v>1423</v>
       </c>
       <c r="D172" s="2">
         <v>4</v>
@@ -7840,7 +7843,7 @@
         <v>151.23106709999999</v>
       </c>
       <c r="C173" s="2">
-        <v>1423</v>
+        <v>2322</v>
       </c>
       <c r="D173" s="2">
         <v>4</v>
@@ -7881,7 +7884,7 @@
         <v>151.23116200000001</v>
       </c>
       <c r="C174" s="2">
-        <v>2322</v>
+        <v>1303</v>
       </c>
       <c r="D174" s="2">
         <v>3</v>
@@ -7922,7 +7925,7 @@
         <v>151.2312349</v>
       </c>
       <c r="C175" s="2">
-        <v>1303</v>
+        <v>1424</v>
       </c>
       <c r="D175" s="2">
         <v>3</v>
@@ -7963,7 +7966,7 @@
         <v>151.23135719999999</v>
       </c>
       <c r="C176" s="2">
-        <v>1424</v>
+        <v>1328</v>
       </c>
       <c r="D176" s="2">
         <v>4</v>
@@ -8004,7 +8007,7 @@
         <v>151.2314696</v>
       </c>
       <c r="C177" s="2">
-        <v>1328</v>
+        <v>10687</v>
       </c>
       <c r="D177" s="2">
         <v>4</v>
@@ -8045,7 +8048,7 @@
         <v>151.23106870000001</v>
       </c>
       <c r="C178" s="2">
-        <v>10687</v>
+        <v>1377</v>
       </c>
       <c r="D178" s="2">
         <v>16</v>
@@ -8086,7 +8089,7 @@
         <v>151.2313029</v>
       </c>
       <c r="C179" s="2">
-        <v>1377</v>
+        <v>13903</v>
       </c>
       <c r="D179" s="2">
         <v>17</v>
@@ -8127,7 +8130,7 @@
         <v>151.23180790000001</v>
       </c>
       <c r="C180" s="2">
-        <v>13903</v>
+        <v>1392</v>
       </c>
       <c r="D180" s="2">
         <v>10</v>
@@ -8168,7 +8171,7 @@
         <v>151.23225070000001</v>
       </c>
       <c r="C181" s="2">
-        <v>1392</v>
+        <v>1430</v>
       </c>
       <c r="D181" s="2">
         <v>11</v>
@@ -8209,7 +8212,7 @@
         <v>151.23223859999999</v>
       </c>
       <c r="C182" s="2">
-        <v>1430</v>
+        <v>1879</v>
       </c>
       <c r="D182" s="2">
         <v>10</v>
@@ -8250,7 +8253,7 @@
         <v>151.23224060000001</v>
       </c>
       <c r="C183" s="2">
-        <v>1879</v>
+        <v>8543</v>
       </c>
       <c r="D183" s="2">
         <v>11</v>
@@ -8291,7 +8294,7 @@
         <v>151.23275709999999</v>
       </c>
       <c r="C184" s="2">
-        <v>8543</v>
+        <v>1319</v>
       </c>
       <c r="D184" s="2">
         <v>13</v>
@@ -8332,7 +8335,7 @@
         <v>151.23279489999999</v>
       </c>
       <c r="C185" s="2">
-        <v>1319</v>
+        <v>1345</v>
       </c>
       <c r="D185" s="2">
         <v>9</v>
@@ -8373,7 +8376,7 @@
         <v>151.23282889999999</v>
       </c>
       <c r="C186" s="2">
-        <v>1345</v>
+        <v>1273</v>
       </c>
       <c r="D186" s="2">
         <v>6</v>
@@ -8414,7 +8417,7 @@
         <v>151.2327727</v>
       </c>
       <c r="C187" s="2">
-        <v>1273</v>
+        <v>1580</v>
       </c>
       <c r="D187" s="2">
         <v>14</v>
@@ -8455,7 +8458,7 @@
         <v>151.2327027</v>
       </c>
       <c r="C188" s="2">
-        <v>1580</v>
+        <v>1287</v>
       </c>
       <c r="D188" s="2">
         <v>9</v>
@@ -8496,7 +8499,7 @@
         <v>151.23274190000001</v>
       </c>
       <c r="C189" s="2">
-        <v>1287</v>
+        <v>1353</v>
       </c>
       <c r="D189" s="2">
         <v>7</v>
@@ -8537,7 +8540,7 @@
         <v>151.23281159999999</v>
       </c>
       <c r="C190" s="2">
-        <v>1353</v>
+        <v>1323</v>
       </c>
       <c r="D190" s="2">
         <v>5</v>
@@ -8578,7 +8581,7 @@
         <v>151.23282270000001</v>
       </c>
       <c r="C191" s="2">
-        <v>1323</v>
+        <v>3395</v>
       </c>
       <c r="D191" s="2">
         <v>5</v>
@@ -8619,7 +8622,7 @@
         <v>151.23290789999999</v>
       </c>
       <c r="C192" s="2">
-        <v>3395</v>
+        <v>1258</v>
       </c>
       <c r="D192" s="2">
         <v>5</v>
@@ -8660,7 +8663,7 @@
         <v>151.23295210000001</v>
       </c>
       <c r="C193" s="2">
-        <v>1258</v>
+        <v>3470</v>
       </c>
       <c r="D193" s="2">
         <v>3</v>
@@ -8701,7 +8704,7 @@
         <v>151.2330207</v>
       </c>
       <c r="C194" s="2">
-        <v>3470</v>
+        <v>1347</v>
       </c>
       <c r="D194" s="2">
         <v>5</v>
@@ -8742,7 +8745,7 @@
         <v>151.23275340000001</v>
       </c>
       <c r="C195" s="2">
-        <v>1347</v>
+        <v>1317</v>
       </c>
       <c r="D195" s="2">
         <v>5</v>
@@ -8783,7 +8786,7 @@
         <v>151.23264990000001</v>
       </c>
       <c r="C196" s="2">
-        <v>1317</v>
+        <v>3390</v>
       </c>
       <c r="D196" s="2">
         <v>23</v>
@@ -8824,7 +8827,7 @@
         <v>151.2327205</v>
       </c>
       <c r="C197" s="2">
-        <v>3390</v>
+        <v>1315</v>
       </c>
       <c r="D197" s="2">
         <v>4</v>
@@ -8865,7 +8868,7 @@
         <v>151.2327305</v>
       </c>
       <c r="C198" s="2">
-        <v>1315</v>
+        <v>1325</v>
       </c>
       <c r="D198" s="2">
         <v>4</v>
@@ -8906,7 +8909,7 @@
         <v>151.2327688</v>
       </c>
       <c r="C199" s="2">
-        <v>1325</v>
+        <v>2310</v>
       </c>
       <c r="D199" s="2">
         <v>4</v>
@@ -8947,7 +8950,7 @@
         <v>151.2329168</v>
       </c>
       <c r="C200" s="2">
-        <v>2310</v>
+        <v>1375</v>
       </c>
       <c r="D200" s="2">
         <v>5</v>
@@ -8988,7 +8991,7 @@
         <v>151.23298439999999</v>
       </c>
       <c r="C201" s="2">
-        <v>1375</v>
+        <v>1272</v>
       </c>
       <c r="D201" s="2">
         <v>5</v>
@@ -9070,7 +9073,7 @@
         <v>151.2330158</v>
       </c>
       <c r="C203" s="2">
-        <v>1272</v>
+        <v>1382</v>
       </c>
       <c r="D203" s="2">
         <v>3</v>
@@ -9111,7 +9114,7 @@
         <v>151.2330503</v>
       </c>
       <c r="C204" s="2">
-        <v>1382</v>
+        <v>1293</v>
       </c>
       <c r="D204" s="2">
         <v>3</v>
@@ -9152,7 +9155,7 @@
         <v>151.2329914</v>
       </c>
       <c r="C205" s="2">
-        <v>1293</v>
+        <v>1343</v>
       </c>
       <c r="D205" s="2">
         <v>8</v>
@@ -9193,7 +9196,7 @@
         <v>151.23300259999999</v>
       </c>
       <c r="C206" s="2">
-        <v>1343</v>
+        <v>1294</v>
       </c>
       <c r="D206" s="2">
         <v>5</v>
@@ -9234,7 +9237,7 @@
         <v>151.23314329999999</v>
       </c>
       <c r="C207" s="2">
-        <v>1294</v>
+        <v>1442</v>
       </c>
       <c r="D207" s="2">
         <v>3</v>
@@ -9275,7 +9278,7 @@
         <v>151.23317700000001</v>
       </c>
       <c r="C208" s="2">
-        <v>1442</v>
+        <v>1276</v>
       </c>
       <c r="D208" s="2">
         <v>5</v>
@@ -9316,7 +9319,7 @@
         <v>151.23317710000001</v>
       </c>
       <c r="C209" s="2">
-        <v>1276</v>
+        <v>1326</v>
       </c>
       <c r="D209" s="2">
         <v>5</v>
@@ -9357,7 +9360,7 @@
         <v>151.23317710000001</v>
       </c>
       <c r="C210" s="2">
-        <v>1326</v>
+        <v>1352</v>
       </c>
       <c r="D210" s="2">
         <v>5</v>
@@ -9398,7 +9401,7 @@
         <v>151.23317710000001</v>
       </c>
       <c r="C211" s="2">
-        <v>1352</v>
+        <v>3386</v>
       </c>
       <c r="D211" s="2">
         <v>5</v>
@@ -9439,7 +9442,7 @@
         <v>151.2331786</v>
       </c>
       <c r="C212" s="2">
-        <v>3386</v>
+        <v>1304</v>
       </c>
       <c r="D212" s="2">
         <v>9</v>
@@ -9480,7 +9483,7 @@
         <v>151.23317850000001</v>
       </c>
       <c r="C213" s="2">
-        <v>1304</v>
+        <v>1323</v>
       </c>
       <c r="D213" s="2">
         <v>10</v>
@@ -9521,7 +9524,7 @@
         <v>151.23318399999999</v>
       </c>
       <c r="C214" s="2">
-        <v>1323</v>
+        <v>1357</v>
       </c>
       <c r="D214" s="2">
         <v>4</v>
@@ -9562,7 +9565,7 @@
         <v>151.23318399999999</v>
       </c>
       <c r="C215" s="2">
-        <v>1357</v>
+        <v>1387</v>
       </c>
       <c r="D215" s="2">
         <v>4</v>
@@ -9603,7 +9606,7 @@
         <v>151.2334625</v>
       </c>
       <c r="C216" s="2">
-        <v>1387</v>
+        <v>1309</v>
       </c>
       <c r="D216" s="2">
         <v>14</v>
@@ -9644,7 +9647,7 @@
         <v>151.23336520000001</v>
       </c>
       <c r="C217" s="2">
-        <v>1309</v>
+        <v>1321</v>
       </c>
       <c r="D217" s="2">
         <v>4</v>
@@ -9685,7 +9688,7 @@
         <v>151.23349279999999</v>
       </c>
       <c r="C218" s="2">
-        <v>1321</v>
+        <v>1290</v>
       </c>
       <c r="D218" s="2">
         <v>3</v>
@@ -9726,7 +9729,7 @@
         <v>151.2338115</v>
       </c>
       <c r="C219" s="2">
-        <v>1290</v>
+        <v>1396</v>
       </c>
       <c r="D219" s="2">
         <v>4</v>
@@ -9767,7 +9770,7 @@
         <v>151.2338115</v>
       </c>
       <c r="C220" s="2">
-        <v>1396</v>
+        <v>1410</v>
       </c>
       <c r="D220" s="2">
         <v>4</v>
@@ -9808,7 +9811,7 @@
         <v>151.23383419999999</v>
       </c>
       <c r="C221" s="2">
-        <v>1410</v>
+        <v>4398</v>
       </c>
       <c r="D221" s="2">
         <v>4</v>
@@ -9849,7 +9852,7 @@
         <v>151.23383419999999</v>
       </c>
       <c r="C222" s="2">
-        <v>4398</v>
+        <v>4634</v>
       </c>
       <c r="D222" s="2">
         <v>4</v>
@@ -9890,7 +9893,7 @@
         <v>151.23387289999999</v>
       </c>
       <c r="C223" s="2">
-        <v>4634</v>
+        <v>1263</v>
       </c>
       <c r="D223" s="2">
         <v>9</v>
@@ -9931,7 +9934,7 @@
         <v>151.2335137</v>
       </c>
       <c r="C224" s="2">
-        <v>1263</v>
+        <v>1303</v>
       </c>
       <c r="D224" s="2">
         <v>21.666</v>
@@ -9972,7 +9975,7 @@
         <v>151.23316070000001</v>
       </c>
       <c r="C225" s="2">
-        <v>1303</v>
+        <v>3342</v>
       </c>
       <c r="D225" s="2">
         <v>21.039000000000001</v>
@@ -10013,7 +10016,7 @@
         <v>151.23316070000001</v>
       </c>
       <c r="C226" s="2">
-        <v>3342</v>
+        <v>1277</v>
       </c>
       <c r="D226" s="2">
         <v>21.039000000000001</v>
@@ -10054,7 +10057,7 @@
         <v>151.23343399999999</v>
       </c>
       <c r="C227" s="2">
-        <v>1277</v>
+        <v>1275</v>
       </c>
       <c r="D227" s="2">
         <v>22.067</v>
@@ -10095,7 +10098,7 @@
         <v>151.23343399999999</v>
       </c>
       <c r="C228" s="2">
-        <v>1275</v>
+        <v>1281</v>
       </c>
       <c r="D228" s="2">
         <v>22.067</v>
@@ -10136,7 +10139,7 @@
         <v>151.23341120000001</v>
       </c>
       <c r="C229" s="2">
-        <v>1281</v>
+        <v>31441</v>
       </c>
       <c r="D229" s="2">
         <v>21.641999999999999</v>
@@ -10177,7 +10180,7 @@
         <v>151.23393490000001</v>
       </c>
       <c r="C230" s="2">
-        <v>31441</v>
+        <v>2320</v>
       </c>
       <c r="D230" s="2">
         <v>21.649000000000001</v>
@@ -10218,7 +10221,7 @@
         <v>151.23363889999999</v>
       </c>
       <c r="C231" s="2">
-        <v>2320</v>
+        <v>1240</v>
       </c>
       <c r="D231" s="2">
         <v>22.120999999999999</v>
@@ -10259,7 +10262,7 @@
         <v>151.23368439999999</v>
       </c>
       <c r="C232" s="2">
-        <v>1240</v>
+        <v>1366</v>
       </c>
       <c r="D232" s="2">
         <v>22.137</v>
@@ -10300,7 +10303,7 @@
         <v>151.23391409999999</v>
       </c>
       <c r="C233" s="2">
-        <v>1366</v>
+        <v>1298</v>
       </c>
       <c r="D233" s="2">
         <v>3</v>
@@ -10341,7 +10344,7 @@
         <v>151.2339322</v>
       </c>
       <c r="C234" s="2">
-        <v>1298</v>
+        <v>1377</v>
       </c>
       <c r="D234" s="2">
         <v>3</v>
@@ -10382,7 +10385,7 @@
         <v>151.23391240000001</v>
       </c>
       <c r="C235" s="2">
-        <v>1377</v>
+        <v>3475</v>
       </c>
       <c r="D235" s="2">
         <v>3</v>
@@ -10423,7 +10426,7 @@
         <v>151.2339193</v>
       </c>
       <c r="C236" s="2">
-        <v>3475</v>
+        <v>2065</v>
       </c>
       <c r="D236" s="2">
         <v>3</v>
@@ -10464,7 +10467,7 @@
         <v>151.23392770000001</v>
       </c>
       <c r="C237" s="2">
-        <v>2065</v>
+        <v>3421</v>
       </c>
       <c r="D237" s="2">
         <v>3</v>
@@ -10505,7 +10508,7 @@
         <v>151.2339193</v>
       </c>
       <c r="C238" s="2">
-        <v>3421</v>
+        <v>3460</v>
       </c>
       <c r="D238" s="2">
         <v>3</v>
@@ -10546,7 +10549,7 @@
         <v>151.23396030000001</v>
       </c>
       <c r="C239" s="2">
-        <v>3460</v>
+        <v>1336</v>
       </c>
       <c r="D239" s="2">
         <v>4</v>
@@ -10587,7 +10590,7 @@
         <v>151.23396030000001</v>
       </c>
       <c r="C240" s="2">
-        <v>1336</v>
+        <v>1363</v>
       </c>
       <c r="D240" s="2">
         <v>4</v>
@@ -10628,7 +10631,7 @@
         <v>151.2339715</v>
       </c>
       <c r="C241" s="2">
-        <v>1363</v>
+        <v>2064</v>
       </c>
       <c r="D241" s="2">
         <v>3</v>
@@ -10669,7 +10672,7 @@
         <v>151.2339715</v>
       </c>
       <c r="C242" s="2">
-        <v>2064</v>
+        <v>3405</v>
       </c>
       <c r="D242" s="2">
         <v>3</v>
@@ -10710,7 +10713,7 @@
         <v>151.2340026</v>
       </c>
       <c r="C243" s="2">
-        <v>3405</v>
+        <v>4139</v>
       </c>
       <c r="D243" s="2">
         <v>4</v>
@@ -10751,7 +10754,7 @@
         <v>151.2340026</v>
       </c>
       <c r="C244" s="2">
-        <v>4139</v>
+        <v>4140</v>
       </c>
       <c r="D244" s="2">
         <v>4</v>
@@ -10792,7 +10795,7 @@
         <v>151.23356419999999</v>
       </c>
       <c r="C245" s="2">
-        <v>4140</v>
+        <v>1286</v>
       </c>
       <c r="D245" s="2">
         <v>13</v>
@@ -10833,7 +10836,7 @@
         <v>151.23356419999999</v>
       </c>
       <c r="C246" s="2">
-        <v>1286</v>
+        <v>1261</v>
       </c>
       <c r="D246" s="2">
         <v>13</v>
@@ -10874,7 +10877,7 @@
         <v>151.23303179999999</v>
       </c>
       <c r="C247" s="2">
-        <v>1261</v>
+        <v>6094</v>
       </c>
       <c r="D247" s="2">
         <v>12</v>
@@ -10913,7 +10916,7 @@
         <v>151.23303179999999</v>
       </c>
       <c r="C248" s="2">
-        <v>6094</v>
+        <v>6231</v>
       </c>
       <c r="D248" s="2">
         <v>12</v>
@@ -10952,7 +10955,7 @@
         <v>151.23255030000001</v>
       </c>
       <c r="C249" s="2">
-        <v>6231</v>
+        <v>1997</v>
       </c>
       <c r="D249" s="2">
         <v>4</v>
@@ -10993,7 +10996,7 @@
         <v>151.23303179999999</v>
       </c>
       <c r="C250" s="2">
-        <v>1997</v>
+        <v>55192</v>
       </c>
       <c r="D250" s="2">
         <v>12</v>
@@ -11034,7 +11037,7 @@
         <v>151.23255599999999</v>
       </c>
       <c r="C251" s="2">
-        <v>55192</v>
+        <v>1216</v>
       </c>
       <c r="D251" s="2">
         <v>4</v>
@@ -11073,7 +11076,7 @@
         <v>151.23255599999999</v>
       </c>
       <c r="C252" s="2">
-        <v>1216</v>
+        <v>1221</v>
       </c>
       <c r="D252" s="2">
         <v>4</v>
@@ -11112,7 +11115,7 @@
         <v>151.23302960000001</v>
       </c>
       <c r="C253" s="2">
-        <v>1221</v>
+        <v>1410</v>
       </c>
       <c r="D253" s="2">
         <v>3</v>
@@ -11153,7 +11156,7 @@
         <v>151.23302960000001</v>
       </c>
       <c r="C254" s="2">
-        <v>1410</v>
+        <v>1255</v>
       </c>
       <c r="D254" s="2">
         <v>3</v>
@@ -11194,7 +11197,7 @@
         <v>151.23309689999999</v>
       </c>
       <c r="C255" s="2">
-        <v>1255</v>
+        <v>10090</v>
       </c>
       <c r="D255" s="2">
         <v>3</v>
@@ -11235,7 +11238,7 @@
         <v>151.23309689999999</v>
       </c>
       <c r="C256" s="2">
-        <v>10090</v>
+        <v>10207</v>
       </c>
       <c r="D256" s="2">
         <v>3</v>
@@ -11276,7 +11279,7 @@
         <v>151.23309689999999</v>
       </c>
       <c r="C257" s="2">
-        <v>10207</v>
+        <v>9605</v>
       </c>
       <c r="D257" s="2">
         <v>3</v>
@@ -11317,7 +11320,7 @@
         <v>151.23311100000001</v>
       </c>
       <c r="C258" s="2">
-        <v>9605</v>
+        <v>2329</v>
       </c>
       <c r="D258" s="2">
         <v>3</v>
@@ -11358,7 +11361,7 @@
         <v>151.23311100000001</v>
       </c>
       <c r="C259" s="2">
-        <v>2329</v>
+        <v>2375</v>
       </c>
       <c r="D259" s="2">
         <v>3</v>
@@ -11399,7 +11402,7 @@
         <v>151.23311100000001</v>
       </c>
       <c r="C260" s="2">
-        <v>2375</v>
+        <v>3482</v>
       </c>
       <c r="D260" s="2">
         <v>3</v>
@@ -11440,7 +11443,7 @@
         <v>151.2331835</v>
       </c>
       <c r="C261" s="2">
-        <v>3482</v>
+        <v>1278</v>
       </c>
       <c r="D261" s="2">
         <v>22.475000000000001</v>
@@ -11481,7 +11484,7 @@
         <v>151.2331835</v>
       </c>
       <c r="C262" s="2">
-        <v>1278</v>
+        <v>1272</v>
       </c>
       <c r="D262" s="2">
         <v>22.475000000000001</v>
@@ -11522,7 +11525,7 @@
         <v>151.2331835</v>
       </c>
       <c r="C263" s="2">
-        <v>1272</v>
+        <v>1243</v>
       </c>
       <c r="D263" s="2">
         <v>22.475000000000001</v>
@@ -11563,7 +11566,7 @@
         <v>151.23352510000001</v>
       </c>
       <c r="C264" s="2">
-        <v>1243</v>
+        <v>2350</v>
       </c>
       <c r="D264" s="2">
         <v>21.302</v>
@@ -11604,7 +11607,7 @@
         <v>151.23352510000001</v>
       </c>
       <c r="C265" s="2">
-        <v>2350</v>
+        <v>3362</v>
       </c>
       <c r="D265" s="2">
         <v>21.302</v>
@@ -11645,7 +11648,7 @@
         <v>151.23352510000001</v>
       </c>
       <c r="C266" s="2">
-        <v>3362</v>
+        <v>4361</v>
       </c>
       <c r="D266" s="2">
         <v>21.302</v>
@@ -11686,7 +11689,7 @@
         <v>151.2337086</v>
       </c>
       <c r="C267" s="2">
-        <v>4361</v>
+        <v>1262</v>
       </c>
       <c r="D267" s="2">
         <v>3</v>
@@ -11727,7 +11730,7 @@
         <v>151.23369640000001</v>
       </c>
       <c r="C268" s="2">
-        <v>1262</v>
+        <v>1398</v>
       </c>
       <c r="D268" s="2">
         <v>4</v>
@@ -11768,7 +11771,7 @@
         <v>151.2336827</v>
       </c>
       <c r="C269" s="2">
-        <v>1398</v>
+        <v>3325</v>
       </c>
       <c r="D269" s="2">
         <v>3</v>
@@ -11850,7 +11853,7 @@
         <v>151.23378439999999</v>
       </c>
       <c r="C271" s="2">
-        <v>3325</v>
+        <v>37946</v>
       </c>
       <c r="D271" s="2">
         <v>3</v>
@@ -11889,7 +11892,7 @@
         <v>151.2338057</v>
       </c>
       <c r="C272" s="2">
-        <v>37946</v>
+        <v>36932</v>
       </c>
       <c r="D272" s="2">
         <v>3</v>
@@ -11928,7 +11931,7 @@
         <v>151.2345004</v>
       </c>
       <c r="C273" s="2">
-        <v>36932</v>
+        <v>1814</v>
       </c>
       <c r="D273" s="2">
         <v>8</v>
@@ -11969,7 +11972,7 @@
         <v>151.2338057</v>
       </c>
       <c r="C274" s="2">
-        <v>1814</v>
+        <v>79092</v>
       </c>
       <c r="D274" s="2">
         <v>3</v>
@@ -12010,7 +12013,7 @@
         <v>151.23480960000001</v>
       </c>
       <c r="C275" s="2">
-        <v>79092</v>
+        <v>1280</v>
       </c>
       <c r="D275" s="2">
         <v>3</v>
@@ -12049,7 +12052,7 @@
         <v>151.23478840000001</v>
       </c>
       <c r="C276" s="2">
-        <v>1280</v>
+        <v>2031</v>
       </c>
       <c r="D276" s="2">
         <v>4</v>
@@ -12090,7 +12093,7 @@
         <v>151.23478019999999</v>
       </c>
       <c r="C277" s="2">
-        <v>2031</v>
+        <v>1351</v>
       </c>
       <c r="D277" s="2">
         <v>4</v>
@@ -12129,7 +12132,7 @@
         <v>151.2346704</v>
       </c>
       <c r="C278" s="2">
-        <v>1351</v>
+        <v>1316</v>
       </c>
       <c r="D278" s="2">
         <v>4</v>
@@ -12170,7 +12173,7 @@
         <v>151.23426000000001</v>
       </c>
       <c r="C279" s="2">
-        <v>1316</v>
+        <v>1330</v>
       </c>
       <c r="D279" s="2">
         <v>6</v>
@@ -12211,7 +12214,7 @@
         <v>151.23414980000001</v>
       </c>
       <c r="C280" s="2">
-        <v>1330</v>
+        <v>1369</v>
       </c>
       <c r="D280" s="2">
         <v>9</v>
@@ -12252,7 +12255,7 @@
         <v>151.2342362</v>
       </c>
       <c r="C281" s="2">
-        <v>1369</v>
+        <v>1378</v>
       </c>
       <c r="D281" s="2">
         <v>11</v>
@@ -12293,7 +12296,7 @@
         <v>151.23428680000001</v>
       </c>
       <c r="C282" s="2">
-        <v>1378</v>
+        <v>1417</v>
       </c>
       <c r="D282" s="2">
         <v>9</v>
@@ -12334,7 +12337,7 @@
         <v>151.23429970000001</v>
       </c>
       <c r="C283" s="2">
-        <v>1417</v>
+        <v>1264</v>
       </c>
       <c r="D283" s="2">
         <v>11</v>
@@ -12375,7 +12378,7 @@
         <v>151.2343113</v>
       </c>
       <c r="C284" s="2">
-        <v>1264</v>
+        <v>1268</v>
       </c>
       <c r="D284" s="2">
         <v>12</v>
@@ -12416,7 +12419,7 @@
         <v>151.23450740000001</v>
       </c>
       <c r="C285" s="2">
-        <v>1268</v>
+        <v>1362</v>
       </c>
       <c r="D285" s="2">
         <v>12</v>
@@ -12457,7 +12460,7 @@
         <v>151.23464419999999</v>
       </c>
       <c r="C286" s="2">
-        <v>1362</v>
+        <v>4520</v>
       </c>
       <c r="D286" s="2">
         <v>9</v>
@@ -12498,7 +12501,7 @@
         <v>151.23464419999999</v>
       </c>
       <c r="C287" s="2">
-        <v>4520</v>
+        <v>6353</v>
       </c>
       <c r="D287" s="2">
         <v>9</v>
@@ -12539,7 +12542,7 @@
         <v>151.2347422</v>
       </c>
       <c r="C288" s="2">
-        <v>6353</v>
+        <v>1417</v>
       </c>
       <c r="D288" s="2">
         <v>8</v>
@@ -12580,7 +12583,7 @@
         <v>151.23448719999999</v>
       </c>
       <c r="C289" s="2">
-        <v>1417</v>
+        <v>1325</v>
       </c>
       <c r="D289" s="2">
         <v>16</v>
@@ -12621,7 +12624,7 @@
         <v>151.23439329999999</v>
       </c>
       <c r="C290" s="2">
-        <v>1325</v>
+        <v>3376</v>
       </c>
       <c r="D290" s="2">
         <v>15</v>
@@ -12662,7 +12665,7 @@
         <v>151.23433370000001</v>
       </c>
       <c r="C291" s="2">
-        <v>3376</v>
+        <v>1386</v>
       </c>
       <c r="D291" s="2">
         <v>10</v>
@@ -12703,7 +12706,7 @@
         <v>151.2342051</v>
       </c>
       <c r="C292" s="2">
-        <v>1386</v>
+        <v>1708</v>
       </c>
       <c r="D292" s="2">
         <v>6</v>
@@ -12744,7 +12747,7 @@
         <v>151.23429400000001</v>
       </c>
       <c r="C293" s="2">
-        <v>1708</v>
+        <v>3459</v>
       </c>
       <c r="D293" s="2">
         <v>9</v>
@@ -12785,7 +12788,7 @@
         <v>151.2342458</v>
       </c>
       <c r="C294" s="2">
-        <v>3459</v>
+        <v>1616</v>
       </c>
       <c r="D294" s="2">
         <v>4</v>
@@ -12826,7 +12829,7 @@
         <v>151.2342314</v>
       </c>
       <c r="C295" s="2">
-        <v>1616</v>
+        <v>1329</v>
       </c>
       <c r="D295" s="2">
         <v>4</v>
@@ -12867,7 +12870,7 @@
         <v>151.23434850000001</v>
       </c>
       <c r="C296" s="2">
-        <v>1329</v>
+        <v>1911</v>
       </c>
       <c r="D296" s="2">
         <v>3</v>
@@ -12908,7 +12911,7 @@
         <v>151.23445910000001</v>
       </c>
       <c r="C297" s="2">
-        <v>1911</v>
+        <v>1401</v>
       </c>
       <c r="D297" s="2">
         <v>3</v>
@@ -12949,7 +12952,7 @@
         <v>151.23450980000001</v>
       </c>
       <c r="C298" s="2">
-        <v>1401</v>
+        <v>1413</v>
       </c>
       <c r="D298" s="2">
         <v>3</v>
@@ -12990,7 +12993,7 @@
         <v>151.2345828</v>
       </c>
       <c r="C299" s="2">
-        <v>1413</v>
+        <v>3622</v>
       </c>
       <c r="D299" s="2">
         <v>5</v>
@@ -13031,7 +13034,7 @@
         <v>151.23475500000001</v>
       </c>
       <c r="C300" s="2">
-        <v>3622</v>
+        <v>1340</v>
       </c>
       <c r="D300" s="2">
         <v>4</v>
@@ -13072,7 +13075,7 @@
         <v>151.23475500000001</v>
       </c>
       <c r="C301" s="2">
-        <v>1340</v>
+        <v>1353</v>
       </c>
       <c r="D301" s="2">
         <v>4</v>
@@ -13113,7 +13116,7 @@
         <v>151.2350764</v>
       </c>
       <c r="C302" s="2">
-        <v>1353</v>
+        <v>1380</v>
       </c>
       <c r="D302" s="2">
         <v>4</v>
@@ -13154,7 +13157,7 @@
         <v>151.23509189999999</v>
       </c>
       <c r="C303" s="2">
-        <v>1380</v>
+        <v>1327</v>
       </c>
       <c r="D303" s="2">
         <v>5</v>
@@ -13195,7 +13198,7 @@
         <v>151.23529669999999</v>
       </c>
       <c r="C304" s="2">
-        <v>1327</v>
+        <v>1526</v>
       </c>
       <c r="D304" s="2">
         <v>6</v>
@@ -13236,7 +13239,7 @@
         <v>151.23521529999999</v>
       </c>
       <c r="C305" s="2">
-        <v>1526</v>
+        <v>1329</v>
       </c>
       <c r="D305" s="2">
         <v>14</v>
@@ -13277,7 +13280,7 @@
         <v>151.23521529999999</v>
       </c>
       <c r="C306" s="2">
-        <v>1329</v>
+        <v>1319</v>
       </c>
       <c r="D306" s="2">
         <v>14</v>
@@ -13318,7 +13321,7 @@
         <v>151.23521529999999</v>
       </c>
       <c r="C307" s="2">
-        <v>1319</v>
+        <v>1336</v>
       </c>
       <c r="D307" s="2">
         <v>14</v>
@@ -13359,7 +13362,7 @@
         <v>151.23581859999999</v>
       </c>
       <c r="C308" s="2">
-        <v>1336</v>
+        <v>20100</v>
       </c>
       <c r="D308" s="2">
         <v>11</v>
@@ -13400,7 +13403,7 @@
         <v>151.23581859999999</v>
       </c>
       <c r="C309" s="2">
-        <v>20100</v>
+        <v>21091</v>
       </c>
       <c r="D309" s="2">
         <v>11</v>
@@ -13441,7 +13444,7 @@
         <v>151.23581859999999</v>
       </c>
       <c r="C310" s="2">
-        <v>21091</v>
+        <v>21041</v>
       </c>
       <c r="D310" s="2">
         <v>11</v>
@@ -13482,7 +13485,7 @@
         <v>151.2361172</v>
       </c>
       <c r="C311" s="2">
-        <v>21041</v>
+        <v>2543</v>
       </c>
       <c r="D311" s="2">
         <v>3</v>
@@ -13523,7 +13526,7 @@
         <v>151.2361172</v>
       </c>
       <c r="C312" s="2">
-        <v>2543</v>
+        <v>2577</v>
       </c>
       <c r="D312" s="2">
         <v>3</v>
@@ -13564,7 +13567,7 @@
         <v>151.2361172</v>
       </c>
       <c r="C313" s="2">
-        <v>2577</v>
+        <v>3114</v>
       </c>
       <c r="D313" s="2">
         <v>3</v>
@@ -13605,7 +13608,7 @@
         <v>151.2361903</v>
       </c>
       <c r="C314" s="2">
-        <v>3114</v>
+        <v>2304</v>
       </c>
       <c r="D314" s="2">
         <v>4</v>
@@ -13646,7 +13649,7 @@
         <v>151.2361903</v>
       </c>
       <c r="C315" s="2">
-        <v>2304</v>
+        <v>2620</v>
       </c>
       <c r="D315" s="2">
         <v>4</v>
@@ -13687,7 +13690,7 @@
         <v>151.2363268</v>
       </c>
       <c r="C316" s="2">
-        <v>2620</v>
+        <v>21569</v>
       </c>
       <c r="D316" s="2">
         <v>3</v>
@@ -13726,7 +13729,7 @@
         <v>151.2363268</v>
       </c>
       <c r="C317" s="2">
-        <v>21569</v>
+        <v>21546</v>
       </c>
       <c r="D317" s="2">
         <v>3</v>
@@ -13765,7 +13768,7 @@
         <v>151.2362981</v>
       </c>
       <c r="C318" s="2">
-        <v>21546</v>
+        <v>2053</v>
       </c>
       <c r="D318" s="2">
         <v>4</v>
@@ -13806,7 +13809,7 @@
         <v>151.2363268</v>
       </c>
       <c r="C319" s="2">
-        <v>2053</v>
+        <v>132644</v>
       </c>
       <c r="D319" s="2">
         <v>3</v>
@@ -13847,7 +13850,7 @@
         <v>151.2362444</v>
       </c>
       <c r="C320" s="2">
-        <v>132644</v>
+        <v>20996</v>
       </c>
       <c r="D320" s="2">
         <v>4</v>
@@ -13888,7 +13891,7 @@
         <v>151.2362147</v>
       </c>
       <c r="C321" s="2">
-        <v>20996</v>
+        <v>18991</v>
       </c>
       <c r="D321" s="2">
         <v>4</v>
@@ -13927,7 +13930,7 @@
         <v>151.2362147</v>
       </c>
       <c r="C322" s="2">
-        <v>18991</v>
+        <v>19062</v>
       </c>
       <c r="D322" s="2">
         <v>4</v>
@@ -13966,7 +13969,7 @@
         <v>151.23596610000001</v>
       </c>
       <c r="C323" s="2">
-        <v>19062</v>
+        <v>2481</v>
       </c>
       <c r="D323" s="2">
         <v>4</v>
@@ -14007,7 +14010,7 @@
         <v>151.23596610000001</v>
       </c>
       <c r="C324" s="2">
-        <v>2481</v>
+        <v>2449</v>
       </c>
       <c r="D324" s="2">
         <v>4</v>
@@ -14048,7 +14051,7 @@
         <v>151.23596610000001</v>
       </c>
       <c r="C325" s="2">
-        <v>2449</v>
+        <v>2481</v>
       </c>
       <c r="D325" s="2">
         <v>4</v>
@@ -14089,7 +14092,7 @@
         <v>151.23588480000001</v>
       </c>
       <c r="C326" s="2">
-        <v>2481</v>
+        <v>52178</v>
       </c>
       <c r="D326" s="2">
         <v>4</v>
@@ -14130,7 +14133,7 @@
         <v>151.23584500000001</v>
       </c>
       <c r="C327" s="2">
-        <v>52178</v>
+        <v>51563</v>
       </c>
       <c r="D327" s="2">
         <v>5</v>
@@ -14171,7 +14174,7 @@
         <v>151.23553580000001</v>
       </c>
       <c r="C328" s="2">
-        <v>51563</v>
+        <v>27461</v>
       </c>
       <c r="D328" s="2">
         <v>3</v>
@@ -14212,7 +14215,7 @@
         <v>151.2348896</v>
       </c>
       <c r="C329" s="2">
-        <v>27461</v>
+        <v>3664</v>
       </c>
       <c r="D329" s="2">
         <v>3</v>
@@ -14251,7 +14254,7 @@
         <v>151.2348896</v>
       </c>
       <c r="C330" s="2">
-        <v>3664</v>
+        <v>3514</v>
       </c>
       <c r="D330" s="2">
         <v>3</v>
@@ -14290,7 +14293,7 @@
         <v>151.23454939999999</v>
       </c>
       <c r="C331" s="2">
-        <v>3514</v>
+        <v>1965</v>
       </c>
       <c r="D331" s="2">
         <v>6</v>
@@ -14331,7 +14334,7 @@
         <v>151.2348896</v>
       </c>
       <c r="C332" s="2">
-        <v>1965</v>
+        <v>116103</v>
       </c>
       <c r="D332" s="2">
         <v>3</v>
@@ -14372,7 +14375,7 @@
         <v>151.23453040000001</v>
       </c>
       <c r="C333" s="2">
-        <v>116103</v>
+        <v>1706</v>
       </c>
       <c r="D333" s="2">
         <v>5</v>
@@ -14411,7 +14414,7 @@
         <v>151.23441009999999</v>
       </c>
       <c r="C334" s="2">
-        <v>1706</v>
+        <v>1423</v>
       </c>
       <c r="D334" s="2">
         <v>3</v>
@@ -14450,7 +14453,7 @@
         <v>151.2342898</v>
       </c>
       <c r="C335" s="2">
-        <v>1423</v>
+        <v>1442</v>
       </c>
       <c r="D335" s="2">
         <v>9</v>
@@ -14491,7 +14494,7 @@
         <v>151.2342898</v>
       </c>
       <c r="C336" s="2">
-        <v>1442</v>
+        <v>1518</v>
       </c>
       <c r="D336" s="2">
         <v>9</v>
@@ -14532,7 +14535,7 @@
         <v>151.2342898</v>
       </c>
       <c r="C337" s="2">
-        <v>1518</v>
+        <v>1351</v>
       </c>
       <c r="D337" s="2">
         <v>9</v>
@@ -14573,7 +14576,7 @@
         <v>151.23387779999999</v>
       </c>
       <c r="C338" s="2">
-        <v>1351</v>
+        <v>9733</v>
       </c>
       <c r="D338" s="2">
         <v>10</v>
@@ -14614,7 +14617,7 @@
         <v>151.23387779999999</v>
       </c>
       <c r="C339" s="2">
-        <v>9733</v>
+        <v>9731</v>
       </c>
       <c r="D339" s="2">
         <v>10</v>
@@ -14655,7 +14658,7 @@
         <v>151.23387779999999</v>
       </c>
       <c r="C340" s="2">
-        <v>9731</v>
+        <v>9720</v>
       </c>
       <c r="D340" s="2">
         <v>10</v>
@@ -14696,7 +14699,7 @@
         <v>151.2338211</v>
       </c>
       <c r="C341" s="2">
-        <v>9720</v>
+        <v>1417</v>
       </c>
       <c r="D341" s="2">
         <v>8</v>
@@ -14737,7 +14740,7 @@
         <v>151.2338211</v>
       </c>
       <c r="C342" s="2">
-        <v>1417</v>
+        <v>1427</v>
       </c>
       <c r="D342" s="2">
         <v>8</v>
@@ -14778,7 +14781,7 @@
         <v>151.2338211</v>
       </c>
       <c r="C343" s="2">
-        <v>1427</v>
+        <v>1435</v>
       </c>
       <c r="D343" s="2">
         <v>8</v>
@@ -14819,7 +14822,7 @@
         <v>151.2337818</v>
       </c>
       <c r="C344" s="2">
-        <v>1435</v>
+        <v>2037</v>
       </c>
       <c r="D344" s="2">
         <v>8</v>
@@ -14860,7 +14863,7 @@
         <v>151.2337818</v>
       </c>
       <c r="C345" s="2">
-        <v>2037</v>
+        <v>2058</v>
       </c>
       <c r="D345" s="2">
         <v>8</v>
@@ -14901,7 +14904,7 @@
         <v>151.2337818</v>
       </c>
       <c r="C346" s="2">
-        <v>2058</v>
+        <v>2040</v>
       </c>
       <c r="D346" s="2">
         <v>8</v>
@@ -14942,7 +14945,7 @@
         <v>151.23252249999999</v>
       </c>
       <c r="C347" s="2">
-        <v>2040</v>
+        <v>6301</v>
       </c>
       <c r="D347" s="2">
         <v>6</v>
@@ -14983,7 +14986,7 @@
         <v>151.23254890000001</v>
       </c>
       <c r="C348" s="2">
-        <v>6301</v>
+        <v>9265</v>
       </c>
       <c r="D348" s="2">
         <v>6</v>
@@ -15024,7 +15027,7 @@
         <v>151.23252249999999</v>
       </c>
       <c r="C349" s="2">
-        <v>9265</v>
+        <v>6361</v>
       </c>
       <c r="D349" s="2">
         <v>6</v>
@@ -15065,7 +15068,7 @@
         <v>151.23193800000001</v>
       </c>
       <c r="C350" s="2">
-        <v>6361</v>
+        <v>1370</v>
       </c>
       <c r="D350" s="2">
         <v>11</v>
@@ -15106,7 +15109,7 @@
         <v>151.23187229999999</v>
       </c>
       <c r="C351" s="2">
-        <v>1370</v>
+        <v>8454</v>
       </c>
       <c r="D351" s="2">
         <v>10</v>
@@ -15147,7 +15150,7 @@
         <v>151.23187229999999</v>
       </c>
       <c r="C352" s="2">
-        <v>8454</v>
+        <v>8437</v>
       </c>
       <c r="D352" s="2">
         <v>10</v>
@@ -15188,7 +15191,7 @@
         <v>151.2319305</v>
       </c>
       <c r="C353" s="2">
-        <v>8437</v>
+        <v>5696</v>
       </c>
       <c r="D353" s="2">
         <v>14</v>
@@ -15229,7 +15232,7 @@
         <v>151.23217159999999</v>
       </c>
       <c r="C354" s="2">
-        <v>5696</v>
+        <v>5957</v>
       </c>
       <c r="D354" s="2">
         <v>18</v>
@@ -15270,7 +15273,7 @@
         <v>151.2320981</v>
       </c>
       <c r="C355" s="2">
-        <v>5957</v>
+        <v>3863</v>
       </c>
       <c r="D355" s="2">
         <v>17</v>
@@ -15311,7 +15314,7 @@
         <v>151.2320981</v>
       </c>
       <c r="C356" s="2">
-        <v>3863</v>
+        <v>3957</v>
       </c>
       <c r="D356" s="2">
         <v>17</v>
@@ -15352,7 +15355,7 @@
         <v>151.23195480000001</v>
       </c>
       <c r="C357" s="2">
-        <v>3957</v>
+        <v>1530</v>
       </c>
       <c r="D357" s="2">
         <v>14</v>
@@ -15393,7 +15396,7 @@
         <v>151.2318933</v>
       </c>
       <c r="C358" s="2">
-        <v>1530</v>
+        <v>6663</v>
       </c>
       <c r="D358" s="2">
         <v>13</v>
@@ -15434,7 +15437,7 @@
         <v>151.2318933</v>
       </c>
       <c r="C359" s="2">
-        <v>6663</v>
+        <v>6907</v>
       </c>
       <c r="D359" s="2">
         <v>13</v>
@@ -15475,7 +15478,7 @@
         <v>151.2318564</v>
       </c>
       <c r="C360" s="2">
-        <v>6907</v>
+        <v>4449</v>
       </c>
       <c r="D360" s="2">
         <v>12</v>
@@ -15516,7 +15519,7 @@
         <v>151.23188630000001</v>
       </c>
       <c r="C361" s="2">
-        <v>4449</v>
+        <v>11207</v>
       </c>
       <c r="D361" s="2">
         <v>12</v>
@@ -15557,7 +15560,7 @@
         <v>151.2318861</v>
       </c>
       <c r="C362" s="2">
-        <v>11207</v>
+        <v>1640</v>
       </c>
       <c r="D362" s="2">
         <v>11</v>
@@ -15598,7 +15601,7 @@
         <v>151.2318564</v>
       </c>
       <c r="C363" s="2">
-        <v>1640</v>
+        <v>8323</v>
       </c>
       <c r="D363" s="2">
         <v>12</v>
@@ -15639,7 +15642,7 @@
         <v>151.2318789</v>
       </c>
       <c r="C364" s="2">
-        <v>8323</v>
+        <v>1369</v>
       </c>
       <c r="D364" s="2">
         <v>10</v>
@@ -15680,7 +15683,7 @@
         <v>151.2318789</v>
       </c>
       <c r="C365" s="2">
-        <v>1369</v>
+        <v>1886</v>
       </c>
       <c r="D365" s="2">
         <v>10</v>
@@ -15721,7 +15724,7 @@
         <v>151.23186670000001</v>
       </c>
       <c r="C366" s="2">
-        <v>1886</v>
+        <v>1705</v>
       </c>
       <c r="D366" s="2">
         <v>10</v>
@@ -15762,7 +15765,7 @@
         <v>151.23180120000001</v>
       </c>
       <c r="C367" s="2">
-        <v>1705</v>
+        <v>3774</v>
       </c>
       <c r="D367" s="2">
         <v>10</v>
@@ -15803,7 +15806,7 @@
         <v>151.23180120000001</v>
       </c>
       <c r="C368" s="2">
-        <v>3774</v>
+        <v>3905</v>
       </c>
       <c r="D368" s="2">
         <v>10</v>
@@ -15844,7 +15847,7 @@
         <v>151.23180120000001</v>
       </c>
       <c r="C369" s="2">
-        <v>3905</v>
+        <v>4001</v>
       </c>
       <c r="D369" s="2">
         <v>10</v>
@@ -15885,7 +15888,7 @@
         <v>151.2319139</v>
       </c>
       <c r="C370" s="2">
-        <v>4001</v>
+        <v>2036</v>
       </c>
       <c r="D370" s="2">
         <v>7</v>
@@ -15926,7 +15929,7 @@
         <v>151.2319139</v>
       </c>
       <c r="C371" s="2">
-        <v>2036</v>
+        <v>2038</v>
       </c>
       <c r="D371" s="2">
         <v>7</v>
@@ -15967,7 +15970,7 @@
         <v>151.23191990000001</v>
       </c>
       <c r="C372" s="2">
-        <v>2038</v>
+        <v>3660</v>
       </c>
       <c r="D372" s="2">
         <v>8</v>
@@ -16008,7 +16011,7 @@
         <v>151.2319541</v>
       </c>
       <c r="C373" s="2">
-        <v>3660</v>
+        <v>5764</v>
       </c>
       <c r="D373" s="2">
         <v>9</v>
@@ -16049,7 +16052,7 @@
         <v>151.2319541</v>
       </c>
       <c r="C374" s="2">
-        <v>5764</v>
+        <v>5762</v>
       </c>
       <c r="D374" s="2">
         <v>9</v>
@@ -16090,7 +16093,7 @@
         <v>151.23206680000001</v>
       </c>
       <c r="C375" s="2">
-        <v>5762</v>
+        <v>8039</v>
       </c>
       <c r="D375" s="2">
         <v>6</v>
@@ -16131,7 +16134,7 @@
         <v>151.23206680000001</v>
       </c>
       <c r="C376" s="2">
-        <v>8039</v>
+        <v>8055</v>
       </c>
       <c r="D376" s="2">
         <v>6</v>
@@ -16172,7 +16175,7 @@
         <v>151.23206680000001</v>
       </c>
       <c r="C377" s="2">
-        <v>8055</v>
+        <v>8063</v>
       </c>
       <c r="D377" s="2">
         <v>6</v>
@@ -16213,7 +16216,7 @@
         <v>151.23183</v>
       </c>
       <c r="C378" s="2">
-        <v>8063</v>
+        <v>1385</v>
       </c>
       <c r="D378" s="2">
         <v>10</v>
@@ -16254,7 +16257,7 @@
         <v>151.23183</v>
       </c>
       <c r="C379" s="2">
-        <v>1385</v>
+        <v>1440</v>
       </c>
       <c r="D379" s="2">
         <v>10</v>
@@ -16295,7 +16298,7 @@
         <v>151.23183</v>
       </c>
       <c r="C380" s="2">
-        <v>1440</v>
+        <v>1663</v>
       </c>
       <c r="D380" s="2">
         <v>10</v>
@@ -16336,7 +16339,7 @@
         <v>151.23182389999999</v>
       </c>
       <c r="C381" s="2">
-        <v>1663</v>
+        <v>1870</v>
       </c>
       <c r="D381" s="2">
         <v>14</v>
@@ -16377,7 +16380,7 @@
         <v>151.23182389999999</v>
       </c>
       <c r="C382" s="2">
-        <v>1870</v>
+        <v>1871</v>
       </c>
       <c r="D382" s="2">
         <v>14</v>
@@ -16418,7 +16421,7 @@
         <v>151.23182389999999</v>
       </c>
       <c r="C383" s="2">
-        <v>1871</v>
+        <v>1866</v>
       </c>
       <c r="D383" s="2">
         <v>14</v>
@@ -16459,7 +16462,7 @@
         <v>151.231919</v>
       </c>
       <c r="C384" s="2">
-        <v>1866</v>
+        <v>1376</v>
       </c>
       <c r="D384" s="2">
         <v>14</v>
@@ -16500,7 +16503,7 @@
         <v>151.23191679999999</v>
       </c>
       <c r="C385" s="2">
-        <v>1376</v>
+        <v>3419</v>
       </c>
       <c r="D385" s="2">
         <v>14</v>
@@ -16541,7 +16544,7 @@
         <v>151.23191679999999</v>
       </c>
       <c r="C386" s="2">
-        <v>3419</v>
+        <v>3601</v>
       </c>
       <c r="D386" s="2">
         <v>14</v>
@@ -16582,7 +16585,7 @@
         <v>151.23193219999999</v>
       </c>
       <c r="C387" s="2">
-        <v>3601</v>
+        <v>1416</v>
       </c>
       <c r="D387" s="2">
         <v>13</v>
@@ -16623,7 +16626,7 @@
         <v>151.23193219999999</v>
       </c>
       <c r="C388" s="2">
-        <v>1416</v>
+        <v>1407</v>
       </c>
       <c r="D388" s="2">
         <v>13</v>
@@ -16664,7 +16667,7 @@
         <v>151.23193219999999</v>
       </c>
       <c r="C389" s="2">
-        <v>1407</v>
+        <v>1353</v>
       </c>
       <c r="D389" s="2">
         <v>13</v>
@@ -16705,7 +16708,7 @@
         <v>151.2319459</v>
       </c>
       <c r="C390" s="2">
-        <v>1353</v>
+        <v>1464</v>
       </c>
       <c r="D390" s="2">
         <v>13</v>
@@ -16746,7 +16749,7 @@
         <v>151.2319459</v>
       </c>
       <c r="C391" s="2">
-        <v>1464</v>
+        <v>1450</v>
       </c>
       <c r="D391" s="2">
         <v>13</v>
@@ -16787,7 +16790,7 @@
         <v>151.2319459</v>
       </c>
       <c r="C392" s="2">
-        <v>1450</v>
+        <v>1515</v>
       </c>
       <c r="D392" s="2">
         <v>13</v>
@@ -16828,7 +16831,7 @@
         <v>151.2319214</v>
       </c>
       <c r="C393" s="2">
-        <v>1515</v>
+        <v>7710</v>
       </c>
       <c r="D393" s="2">
         <v>13</v>
@@ -16869,7 +16872,7 @@
         <v>151.2319214</v>
       </c>
       <c r="C394" s="2">
-        <v>7710</v>
+        <v>7722</v>
       </c>
       <c r="D394" s="2">
         <v>13</v>
@@ -16910,7 +16913,7 @@
         <v>151.2319214</v>
       </c>
       <c r="C395" s="2">
-        <v>7722</v>
+        <v>7717</v>
       </c>
       <c r="D395" s="2">
         <v>13</v>
@@ -16951,7 +16954,7 @@
         <v>151.23206780000001</v>
       </c>
       <c r="C396" s="2">
-        <v>7717</v>
+        <v>1454</v>
       </c>
       <c r="D396" s="2">
         <v>21.055</v>
@@ -16992,7 +16995,7 @@
         <v>151.23206780000001</v>
       </c>
       <c r="C397" s="2">
-        <v>1454</v>
+        <v>1469</v>
       </c>
       <c r="D397" s="2">
         <v>21.055</v>
@@ -17033,7 +17036,7 @@
         <v>151.2321575</v>
       </c>
       <c r="C398" s="2">
-        <v>1469</v>
+        <v>3356</v>
       </c>
       <c r="D398" s="2">
         <v>14</v>
@@ -17074,7 +17077,7 @@
         <v>151.23213699999999</v>
       </c>
       <c r="C399" s="2">
-        <v>3356</v>
+        <v>1746</v>
       </c>
       <c r="D399" s="2">
         <v>12</v>
@@ -17115,7 +17118,7 @@
         <v>151.23213340000001</v>
       </c>
       <c r="C400" s="2">
-        <v>1746</v>
+        <v>1518</v>
       </c>
       <c r="D400" s="2">
         <v>11</v>
@@ -17156,7 +17159,7 @@
         <v>151.2320713</v>
       </c>
       <c r="C401" s="2">
-        <v>1518</v>
+        <v>1307</v>
       </c>
       <c r="D401" s="2">
         <v>14</v>
@@ -17197,7 +17200,7 @@
         <v>151.23201359999999</v>
       </c>
       <c r="C402" s="2">
-        <v>1307</v>
+        <v>3845</v>
       </c>
       <c r="D402" s="2">
         <v>18</v>
@@ -17238,7 +17241,7 @@
         <v>151.23204659999999</v>
       </c>
       <c r="C403" s="2">
-        <v>3845</v>
+        <v>4229</v>
       </c>
       <c r="D403" s="2">
         <v>15</v>
@@ -17279,7 +17282,7 @@
         <v>151.23178440000001</v>
       </c>
       <c r="C404" s="2">
-        <v>4229</v>
+        <v>7583</v>
       </c>
       <c r="D404" s="2">
         <v>4</v>
@@ -17320,7 +17323,7 @@
         <v>151.23178440000001</v>
       </c>
       <c r="C405" s="2">
-        <v>7583</v>
+        <v>8581</v>
       </c>
       <c r="D405" s="2">
         <v>4</v>
@@ -17361,7 +17364,7 @@
         <v>151.23178440000001</v>
       </c>
       <c r="C406" s="2">
-        <v>8581</v>
+        <v>8583</v>
       </c>
       <c r="D406" s="2">
         <v>4</v>
@@ -17402,7 +17405,7 @@
         <v>151.23159870000001</v>
       </c>
       <c r="C407" s="2">
-        <v>8583</v>
+        <v>1454</v>
       </c>
       <c r="D407" s="2">
         <v>4</v>
@@ -17443,7 +17446,7 @@
         <v>151.23159870000001</v>
       </c>
       <c r="C408" s="2">
-        <v>1454</v>
+        <v>2628</v>
       </c>
       <c r="D408" s="2">
         <v>4</v>
@@ -17484,7 +17487,7 @@
         <v>151.23159870000001</v>
       </c>
       <c r="C409" s="2">
-        <v>2628</v>
+        <v>2636</v>
       </c>
       <c r="D409" s="2">
         <v>4</v>
@@ -17525,7 +17528,7 @@
         <v>151.2316265</v>
       </c>
       <c r="C410" s="2">
-        <v>2636</v>
+        <v>2517</v>
       </c>
       <c r="D410" s="2">
         <v>6</v>
@@ -17566,7 +17569,7 @@
         <v>151.23161949999999</v>
       </c>
       <c r="C411" s="2">
-        <v>2517</v>
+        <v>4323</v>
       </c>
       <c r="D411" s="2">
         <v>4</v>
@@ -17607,7 +17610,7 @@
         <v>151.23161899999999</v>
       </c>
       <c r="C412" s="2">
-        <v>4323</v>
+        <v>1613</v>
       </c>
       <c r="D412" s="2">
         <v>6</v>
@@ -17648,7 +17651,7 @@
         <v>151.2316084</v>
       </c>
       <c r="C413" s="2">
-        <v>1613</v>
+        <v>1762</v>
       </c>
       <c r="D413" s="2">
         <v>7</v>
@@ -17689,7 +17692,7 @@
         <v>151.2316084</v>
       </c>
       <c r="C414" s="2">
-        <v>1762</v>
+        <v>2356</v>
       </c>
       <c r="D414" s="2">
         <v>7</v>
@@ -17730,7 +17733,7 @@
         <v>151.2316084</v>
       </c>
       <c r="C415" s="2">
-        <v>2356</v>
+        <v>2574</v>
       </c>
       <c r="D415" s="2">
         <v>7</v>
@@ -17771,7 +17774,7 @@
         <v>151.23162339999999</v>
       </c>
       <c r="C416" s="2">
-        <v>2574</v>
+        <v>1409</v>
       </c>
       <c r="D416" s="2">
         <v>6</v>
@@ -17812,7 +17815,7 @@
         <v>151.23162339999999</v>
       </c>
       <c r="C417" s="2">
-        <v>1409</v>
+        <v>1359</v>
       </c>
       <c r="D417" s="2">
         <v>6</v>
@@ -17853,7 +17856,7 @@
         <v>151.23162339999999</v>
       </c>
       <c r="C418" s="2">
-        <v>1359</v>
+        <v>1311</v>
       </c>
       <c r="D418" s="2">
         <v>6</v>
@@ -17894,7 +17897,7 @@
         <v>151.23154270000001</v>
       </c>
       <c r="C419" s="2">
-        <v>1311</v>
+        <v>10649</v>
       </c>
       <c r="D419" s="2">
         <v>4</v>
@@ -17935,7 +17938,7 @@
         <v>151.23154270000001</v>
       </c>
       <c r="C420" s="2">
-        <v>10649</v>
+        <v>9684</v>
       </c>
       <c r="D420" s="2">
         <v>4</v>
@@ -17976,7 +17979,7 @@
         <v>151.23154270000001</v>
       </c>
       <c r="C421" s="2">
-        <v>9684</v>
+        <v>10655</v>
       </c>
       <c r="D421" s="2">
         <v>4</v>
@@ -18017,7 +18020,7 @@
         <v>151.2314058</v>
       </c>
       <c r="C422" s="2">
-        <v>10655</v>
+        <v>2479</v>
       </c>
       <c r="D422" s="2">
         <v>4</v>
@@ -18058,7 +18061,7 @@
         <v>151.2314058</v>
       </c>
       <c r="C423" s="2">
-        <v>2479</v>
+        <v>2441</v>
       </c>
       <c r="D423" s="2">
         <v>4</v>
@@ -18099,7 +18102,7 @@
         <v>151.2314058</v>
       </c>
       <c r="C424" s="2">
-        <v>2441</v>
+        <v>2431</v>
       </c>
       <c r="D424" s="2">
         <v>4</v>
@@ -18135,9 +18138,7 @@
     <row r="425" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A425" s="2"/>
       <c r="B425" s="2"/>
-      <c r="C425" s="2">
-        <v>2431</v>
-      </c>
+      <c r="C425" s="2"/>
       <c r="D425" s="2"/>
       <c r="E425" s="2"/>
       <c r="F425" s="2"/>
@@ -18962,7 +18963,6 @@
     <row r="480" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A480" s="2"/>
       <c r="B480" s="2"/>
-      <c r="C480" s="2"/>
       <c r="D480" s="2"/>
       <c r="E480" s="2"/>
       <c r="F480" s="2"/>
@@ -19005,6 +19005,7 @@
     <row r="483" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A483" s="2"/>
       <c r="B483" s="2"/>
+      <c r="C483" s="2"/>
       <c r="D483" s="2"/>
       <c r="E483" s="2"/>
       <c r="F483" s="2"/>
@@ -19699,7 +19700,6 @@
     <row r="531" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A531" s="2"/>
       <c r="B531" s="2"/>
-      <c r="C531" s="2"/>
       <c r="D531" s="2"/>
       <c r="E531" s="2"/>
       <c r="F531" s="2"/>

</xml_diff>